<commit_message>
ajout looping + SQLS
</commit_message>
<xml_diff>
--- a/BaseDeDonnees/Exo_Merise/ExoMerise2c/1_Biblioteque/BDD_tables.xlsx
+++ b/BaseDeDonnees/Exo_Merise/ExoMerise2c/1_Biblioteque/BDD_tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAknouche\CDA_2210\Exos_CDA_2210\BaseDeDonnees\Exo_Merise\ExoMerise2c\1_Biblioteque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{46A9FE76-4AF3-427C-9648-6A74C755D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E08E8A-9D70-435D-8021-D30FC7900E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Entités</t>
   </si>
@@ -110,15 +110,9 @@
     <t>Clients</t>
   </si>
   <si>
-    <t>Client_num_ad</t>
-  </si>
-  <si>
     <t>Numéro d’adhérent unique au client</t>
   </si>
   <si>
-    <t>VARCHAR (50)</t>
-  </si>
-  <si>
     <t>Client_nom</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>Montant de la caution versée par le client</t>
-  </si>
-  <si>
-    <t>DECIMAL (3,3)</t>
   </si>
   <si>
     <t>Emprunts</t>
@@ -182,11 +173,86 @@
   <si>
     <t>Le prenom de l’auteur du livre</t>
   </si>
+  <si>
+    <t>DECIMAL (5,3)</t>
+  </si>
+  <si>
+    <t>obligatoire, &gt;0</t>
+  </si>
+  <si>
+    <t>Client_num_id</t>
+  </si>
+  <si>
+    <t>INT (11)</t>
+  </si>
+  <si>
+    <t>VARCHAR (100)</t>
+  </si>
+  <si>
+    <t>adresse_id</t>
+  </si>
+  <si>
+    <t>INT(11)</t>
+  </si>
+  <si>
+    <t>identifiant, A.I</t>
+  </si>
+  <si>
+    <t>adresse_numero</t>
+  </si>
+  <si>
+    <t>INT(5)</t>
+  </si>
+  <si>
+    <t>adresse_extension</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>Facultatif</t>
+  </si>
+  <si>
+    <t>adresse_voie</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>adresse_complement</t>
+  </si>
+  <si>
+    <t>adresse_ville</t>
+  </si>
+  <si>
+    <t>adresse_code_postal</t>
+  </si>
+  <si>
+    <t>CHAR(5)</t>
+  </si>
+  <si>
+    <t>adresses</t>
+  </si>
+  <si>
+    <t>auteur_id</t>
+  </si>
+  <si>
+    <t>editeur_id</t>
+  </si>
+  <si>
+    <t>editeur_nom</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>editeurs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,8 +300,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -409,58 +481,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,14 +667,96 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,299 +1071,415 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="35"/>
+      <c r="B21" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B23" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C23" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D23" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E23" s="37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="15" t="s">
+      <c r="F23" s="36"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C24" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D24" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E24" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="15" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C25" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D25" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E25" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="15" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C26" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D26" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E26" s="37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="16" t="s">
+    <row r="27" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C27" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D27" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="E27" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="44"/>
+      <c r="B31" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A15:A16"/>
+  <mergeCells count="6">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modif fichier excel bibliotheque
</commit_message>
<xml_diff>
--- a/BaseDeDonnees/Exo_Merise/ExoMerise2c/1_Biblioteque/BDD_tables.xlsx
+++ b/BaseDeDonnees/Exo_Merise/ExoMerise2c/1_Biblioteque/BDD_tables.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAknouche\CDA_2210\Exos_CDA_2210\BaseDeDonnees\Exo_Merise\ExoMerise2c\1_Biblioteque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matha\Clone_CDA_2210\Exos_CDA_2210\BaseDeDonnees\Exo_Merise\ExoMerise2c\1_Biblioteque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19034A11-D469-4A80-8828-26DD41FA15E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B334D21-2C9A-4840-B147-27DE0960E600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionnaire de donnée" sheetId="1" r:id="rId1"/>
     <sheet name="Dépendances fonctionnelles" sheetId="2" r:id="rId2"/>
+    <sheet name="Règles de gestion" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="99">
   <si>
     <t>Entités</t>
   </si>
@@ -280,6 +281,60 @@
   </si>
   <si>
     <t>client_id</t>
+  </si>
+  <si>
+    <t>--&gt;</t>
+  </si>
+  <si>
+    <t>clilent_nom, client_prenom, client_caution, adresse_id</t>
+  </si>
+  <si>
+    <t>adresse_numero, adresse_extension, adresse_voie, adresse_complement, adresse_ville, adresse_code_postal</t>
+  </si>
+  <si>
+    <t>emprunt_date, emprunt_date_retour, client_id, livre_id</t>
+  </si>
+  <si>
+    <t>auteur_nom, auteur_prenom</t>
+  </si>
+  <si>
+    <t>livre_id</t>
+  </si>
+  <si>
+    <t>livre_titre, livre_date_achat, livre_etat_commentaire, livre_isbn, etat_id</t>
+  </si>
+  <si>
+    <t>Règles de gestion</t>
+  </si>
+  <si>
+    <t>1 client habite à 1 seule adresse</t>
+  </si>
+  <si>
+    <t>1 adresse est habitée par 1 ou plusieurs clients</t>
+  </si>
+  <si>
+    <t>1 emprunt concerne 1 livre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 livre est concerné par 0 ou plusieurs emprunts </t>
+  </si>
+  <si>
+    <t>1 emprunt concerne 1 client</t>
+  </si>
+  <si>
+    <t>1 client est concerné par 0 ou plusieurs emprunts</t>
+  </si>
+  <si>
+    <t>1 auteur écrit 0 ou plusieurs livres</t>
+  </si>
+  <si>
+    <t>1 livre est écrit par 1 ou plusieurs auteurs</t>
+  </si>
+  <si>
+    <t>1 livre est qualifié par 1 seul état</t>
+  </si>
+  <si>
+    <t>1 état qualifie 0 ou plusieurs livres</t>
   </si>
 </sst>
 </file>
@@ -346,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -707,11 +762,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,6 +873,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
@@ -836,76 +952,54 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1222,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
@@ -1236,13 +1330,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1262,7 +1356,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="55" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1279,7 +1373,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1294,7 +1388,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1403,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="10" t="s">
         <v>19</v>
       </c>
@@ -1331,7 +1425,7 @@
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="49" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1346,7 +1440,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="13" t="s">
         <v>41</v>
       </c>
@@ -1359,7 +1453,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1372,7 +1466,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="13" t="s">
         <v>46</v>
       </c>
@@ -1385,7 +1479,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="13" t="s">
         <v>48</v>
       </c>
@@ -1398,7 +1492,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
@@ -1411,7 +1505,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="16" t="s">
         <v>50</v>
       </c>
@@ -1431,24 +1525,24 @@
       <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
@@ -1463,7 +1557,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="10" t="s">
         <v>25</v>
       </c>
@@ -1485,7 +1579,7 @@
       <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="52" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1500,7 +1594,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
@@ -1515,7 +1609,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
@@ -1530,14 +1624,14 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="47" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -1552,7 +1646,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="17" t="s">
         <v>55</v>
       </c>
@@ -1565,17 +1659,17 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="26" t="s">
@@ -1589,71 +1683,71 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="57" t="s">
+      <c r="A28" s="53"/>
+      <c r="B28" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="57" t="s">
+      <c r="A29" s="53"/>
+      <c r="B29" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E29" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="58" t="s">
+      <c r="A30" s="53"/>
+      <c r="B30" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="54" t="s">
+      <c r="E30" s="37" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="59" t="s">
+      <c r="A31" s="54"/>
+      <c r="B31" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="55" t="s">
+      <c r="D31" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="35" t="s">
         <v>74</v>
       </c>
       <c r="C33" s="26" t="s">
@@ -1667,8 +1761,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
-      <c r="B34" s="49" t="s">
+      <c r="A34" s="44"/>
+      <c r="B34" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -1681,12 +1775,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+    <row r="36" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="46"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1707,25 +1801,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E1C734-1D85-4F4E-8D0A-7189F13987F2}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="69"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="72"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="71"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="71"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="71"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7377B6A4-12C9-4772-ADCF-B7A6B4222A4F}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="61"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>